<commit_message>
Adding problem 2 part 3 (draft of visualization)
</commit_message>
<xml_diff>
--- a/data/personal_data_sheet.xlsx
+++ b/data/personal_data_sheet.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/angelalarson/Desktop/coding/R/github/ENVS-193DS_homework-03/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D41EFE4-72EF-BE44-B4C3-66F3AA067AB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{AF94B2A4-3863-EC44-B7BC-403F98BD7383}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2180" yWindow="500" windowWidth="24820" windowHeight="15760" xr2:uid="{2AB9EDF7-452D-DF45-A303-23FF4CA39960}"/>
+    <workbookView minimized="1" xWindow="2180" yWindow="500" windowWidth="24820" windowHeight="15760" xr2:uid="{2AB9EDF7-452D-DF45-A303-23FF4CA39960}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="personal_data_sheet" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -499,7 +499,7 @@
   <dimension ref="A1:T38"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>